<commit_message>
System, Products and API set
</commit_message>
<xml_diff>
--- a/docs/Task breakdown .xlsx
+++ b/docs/Task breakdown .xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Meashured website" sheetId="9" r:id="rId1"/>
     <sheet name="Lamda" sheetId="11" r:id="rId2"/>
     <sheet name="data wrangler" sheetId="10" r:id="rId3"/>
     <sheet name="KBCONFIG DB BREAKDOWN" sheetId="14" r:id="rId4"/>
-    <sheet name="Talend(ETL)" sheetId="12" r:id="rId5"/>
-    <sheet name="Dashboard" sheetId="13" r:id="rId6"/>
-    <sheet name="High level" sheetId="1" r:id="rId7"/>
-    <sheet name="Clickhouse DB design and setup" sheetId="2" r:id="rId8"/>
-    <sheet name="Dashboard and Intervention " sheetId="3" r:id="rId9"/>
-    <sheet name="Connectors and meta data discov" sheetId="5" r:id="rId10"/>
-    <sheet name="Configuration Application" sheetId="4" r:id="rId11"/>
-    <sheet name="Automation of ETL" sheetId="8" r:id="rId12"/>
-    <sheet name="API and Data Imports" sheetId="7" r:id="rId13"/>
+    <sheet name="User" sheetId="15" r:id="rId5"/>
+    <sheet name="Talend(ETL)" sheetId="12" r:id="rId6"/>
+    <sheet name="Dashboard" sheetId="13" r:id="rId7"/>
+    <sheet name="High level" sheetId="1" r:id="rId8"/>
+    <sheet name="Clickhouse DB design and setup" sheetId="2" r:id="rId9"/>
+    <sheet name="Dashboard and Intervention " sheetId="3" r:id="rId10"/>
+    <sheet name="Connectors and meta data discov" sheetId="5" r:id="rId11"/>
+    <sheet name="Configuration Application" sheetId="4" r:id="rId12"/>
+    <sheet name="Automation of ETL" sheetId="8" r:id="rId13"/>
+    <sheet name="API and Data Imports" sheetId="7" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'KBCONFIG DB BREAKDOWN'!$B$3:$B$78</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="367">
   <si>
     <t>Task list</t>
   </si>
@@ -1073,12 +1074,96 @@
   <si>
     <t>After setting up the RULEs,  is  this system process the data, or the Talend will process the data as per rule available? Else Which system will process which rule, as per talend,  the Data transformation, convertion of Dates, Pivoting are already available with them.</t>
   </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email_verified_at</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>remember_token</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>LoginId</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>LoginPassword</t>
+  </si>
+  <si>
+    <t>ActiveDirectory</t>
+  </si>
+  <si>
+    <t>DomainName</t>
+  </si>
+  <si>
+    <t>ClientId</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>CreateUserId</t>
+  </si>
+  <si>
+    <t>CreateDateTime</t>
+  </si>
+  <si>
+    <t>LastChangeUserId</t>
+  </si>
+  <si>
+    <t>LastChangeDateTime</t>
+  </si>
+  <si>
+    <t>EmailId</t>
+  </si>
+  <si>
+    <t>ImageUrl</t>
+  </si>
+  <si>
+    <t>GroupID</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>ClientID</t>
+  </si>
+  <si>
+    <t>guard_name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1168,6 +1253,14 @@
     <font>
       <b/>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1382,7 +1475,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1400,14 +1493,39 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1427,50 +1545,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1482,14 +1557,17 @@
     <xf numFmtId="0" fontId="13" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1497,6 +1575,23 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1726,99 +1821,99 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="40" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="H5" s="26"/>
+      <c r="F5" s="38"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="H6" s="26"/>
+      <c r="F6" s="38"/>
+      <c r="H6" s="41"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="H7" s="26"/>
+      <c r="F7" s="38"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="H8" s="26"/>
+      <c r="F8" s="38"/>
+      <c r="H8" s="41"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="F9" s="23"/>
-      <c r="H9" s="26"/>
+      <c r="D9" s="19"/>
+      <c r="F9" s="38"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="F10" s="23"/>
-      <c r="H10" s="26"/>
+      <c r="D10" s="19"/>
+      <c r="F10" s="38"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="F11" s="23"/>
-      <c r="H11" s="26"/>
+      <c r="D11" s="19"/>
+      <c r="F11" s="38"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="F12" s="24"/>
-      <c r="H12" s="27"/>
+      <c r="D12" s="19"/>
+      <c r="F12" s="39"/>
+      <c r="H12" s="42"/>
     </row>
     <row r="20" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M20" s="21"/>
+      <c r="M20" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1835,6 +1930,90 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2018,7 +2197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2271,7 +2450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2334,7 +2513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2406,63 +2585,63 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="28"/>
+      <c r="D19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2476,7 +2655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
@@ -2489,315 +2668,315 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="51" t="s">
         <v>192</v>
       </c>
-      <c r="G2" s="56"/>
-      <c r="H2" s="57"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="52"/>
     </row>
     <row r="3" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="2:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="25" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="25" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="G6" s="33" t="s">
+      <c r="D6" s="24"/>
+      <c r="G6" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="25" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="23" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="23" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="23" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="23" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="23"/>
     </row>
     <row r="12" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="D13" s="31"/>
+      <c r="D13" s="23"/>
     </row>
     <row r="14" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="D14" s="31"/>
+      <c r="D14" s="23"/>
     </row>
     <row r="15" spans="2:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="23" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="23" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="23" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="23" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="35"/>
-      <c r="B20" s="44" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="36">
+      <c r="A21" s="27">
         <v>1</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="36">
+      <c r="A22" s="27">
         <v>2</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="46"/>
     </row>
     <row r="23" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="35">
+      <c r="A23" s="26">
         <v>3</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="44" t="s">
         <v>196</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="48"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="35">
+      <c r="A24" s="26">
         <v>4</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="46"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="35">
+      <c r="A25" s="26">
         <v>5</v>
       </c>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="48"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="46"/>
     </row>
     <row r="26" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="35">
+      <c r="A26" s="26">
         <v>6</v>
       </c>
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="46"/>
     </row>
     <row r="27" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="35">
+      <c r="A27" s="26">
         <v>7</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="47" t="s">
         <v>338</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="39"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="49"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="35">
+      <c r="A28" s="26">
         <v>8</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="47" t="s">
         <v>337</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="39"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="39"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2808,603 +2987,603 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="52"/>
-    <col min="2" max="2" width="21.5703125" style="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" style="52" customWidth="1"/>
-    <col min="8" max="8" width="17" style="52" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" style="52" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="52"/>
+    <col min="1" max="1" width="9.140625" style="33"/>
+    <col min="2" max="2" width="21.5703125" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" style="33" customWidth="1"/>
+    <col min="8" max="8" width="17" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.42578125" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="54" t="s">
         <v>336</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="I4" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="32" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="G5" s="53" t="s">
+      <c r="G5" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="34" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="34" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="G7" s="53" t="s">
+      <c r="G7" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="I7" s="53" t="s">
+      <c r="I7" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="J7" s="53" t="s">
+      <c r="J7" s="34" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="34" t="s">
         <v>238</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="F8" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="H8" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="J8" s="53" t="s">
+      <c r="J8" s="34" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="53"/>
-      <c r="C9" s="53" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="34" t="s">
         <v>247</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="H9" s="53" t="s">
+      <c r="H9" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="I9" s="53" t="s">
+      <c r="I9" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="J9" s="53" t="s">
+      <c r="J9" s="34" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="53"/>
-      <c r="C10" s="53" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="H10" s="53" t="s">
+      <c r="H10" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="J10" s="53" t="s">
+      <c r="J10" s="34" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="53"/>
-      <c r="C11" s="53" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="34" t="s">
         <v>263</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="E11" s="53" t="s">
+      <c r="E11" s="34" t="s">
         <v>265</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="34" t="s">
         <v>266</v>
       </c>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="H11" s="53" t="s">
+      <c r="H11" s="34" t="s">
         <v>268</v>
       </c>
-      <c r="I11" s="53" t="s">
+      <c r="I11" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="J11" s="53" t="s">
+      <c r="J11" s="34" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="53"/>
-      <c r="C12" s="53" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="D12" s="53" t="s">
+      <c r="D12" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="F12" s="53" t="s">
+      <c r="F12" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="G12" s="53" t="s">
+      <c r="G12" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="H12" s="53" t="s">
+      <c r="H12" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="I12" s="53" t="s">
+      <c r="I12" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="J12" s="53" t="s">
+      <c r="J12" s="34" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="53"/>
-      <c r="C13" s="53" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34" t="s">
         <v>279</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="F13" s="53" t="s">
+      <c r="F13" s="34" t="s">
         <v>282</v>
       </c>
-      <c r="G13" s="53" t="s">
+      <c r="G13" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="H13" s="53" t="s">
+      <c r="H13" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="I13" s="52" t="s">
+      <c r="I13" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="J13" s="53" t="s">
+      <c r="J13" s="34" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34" t="s">
         <v>286</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="E14" s="34" t="s">
         <v>287</v>
       </c>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="G14" s="53" t="s">
+      <c r="G14" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="H14" s="53" t="s">
+      <c r="H14" s="34" t="s">
         <v>290</v>
       </c>
-      <c r="I14" s="52" t="s">
+      <c r="I14" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="J14" s="53" t="s">
+      <c r="J14" s="34" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="53"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="F15" s="53" t="s">
+      <c r="F15" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="G15" s="53" t="s">
+      <c r="G15" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="H15" s="53" t="s">
+      <c r="H15" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="I15" s="53" t="s">
+      <c r="I15" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="J15" s="53" t="s">
+      <c r="J15" s="34" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="E16" s="34" t="s">
         <v>301</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="F16" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="G16" s="53" t="s">
+      <c r="G16" s="34" t="s">
         <v>303</v>
       </c>
-      <c r="H16" s="53" t="s">
+      <c r="H16" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="I16" s="53" t="s">
+      <c r="I16" s="34" t="s">
         <v>305</v>
       </c>
-      <c r="J16" s="53"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34" t="s">
         <v>306</v>
       </c>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53" t="s">
+      <c r="F17" s="34"/>
+      <c r="G17" s="34" t="s">
         <v>308</v>
       </c>
-      <c r="H17" s="53" t="s">
+      <c r="H17" s="34" t="s">
         <v>309</v>
       </c>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53" t="s">
+      <c r="I17" s="34"/>
+      <c r="J17" s="34" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="34" t="s">
         <v>312</v>
       </c>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53" t="s">
+      <c r="F18" s="34"/>
+      <c r="G18" s="34" t="s">
         <v>313</v>
       </c>
-      <c r="H18" s="53" t="s">
+      <c r="H18" s="34" t="s">
         <v>314</v>
       </c>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53" t="s">
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="34" t="s">
         <v>316</v>
       </c>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53" t="s">
+      <c r="F19" s="34"/>
+      <c r="G19" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53" t="s">
+      <c r="F20" s="34"/>
+      <c r="G20" s="34" t="s">
         <v>319</v>
       </c>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53" t="s">
+      <c r="H20" s="34"/>
+      <c r="I20" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="J20" s="53"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="53"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53" t="s">
+      <c r="F21" s="34"/>
+      <c r="G21" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53" t="s">
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34" t="s">
         <v>323</v>
       </c>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53" t="s">
+      <c r="F22" s="34"/>
+      <c r="G22" s="34" t="s">
         <v>324</v>
       </c>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53" t="s">
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53" t="s">
+      <c r="F23" s="34"/>
+      <c r="G23" s="34" t="s">
         <v>326</v>
       </c>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="53"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53" t="s">
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53" t="s">
+      <c r="F24" s="34"/>
+      <c r="G24" s="34" t="s">
         <v>328</v>
       </c>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53" t="s">
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34" t="s">
         <v>329</v>
       </c>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53" t="s">
+      <c r="F25" s="34"/>
+      <c r="G25" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53" t="s">
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53" t="s">
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53" t="s">
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53" t="s">
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34" t="s">
         <v>334</v>
       </c>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53" t="s">
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3415,6 +3594,241 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B3" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="58" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="58" t="s">
+        <v>255</v>
+      </c>
+      <c r="H4" s="58" t="s">
+        <v>263</v>
+      </c>
+      <c r="I4" s="58" t="s">
+        <v>271</v>
+      </c>
+      <c r="J4" s="58" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>363</v>
+      </c>
+      <c r="F5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>364</v>
+      </c>
+      <c r="F6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>365</v>
+      </c>
+      <c r="F7" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>360</v>
+      </c>
+      <c r="F9" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>357</v>
+      </c>
+      <c r="F10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>359</v>
+      </c>
+      <c r="F11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>356</v>
+      </c>
+      <c r="F12" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="F31" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>339</v>
+      </c>
+      <c r="F32" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>340</v>
+      </c>
+      <c r="F33" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>366</v>
+      </c>
+      <c r="F34" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>347</v>
+      </c>
+      <c r="F35" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>348</v>
+      </c>
+      <c r="F36" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>348</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:C13"/>
   <sheetViews>
@@ -3428,31 +3842,31 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="55" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C5" s="34"/>
+      <c r="C5" s="55"/>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C6" s="34"/>
+      <c r="C6" s="55"/>
     </row>
     <row r="7" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C7" s="34"/>
+      <c r="C7" s="55"/>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="25" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="30" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="13" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="31" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3464,7 +3878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E12"/>
   <sheetViews>
@@ -3475,56 +3889,56 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="43"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3534,7 +3948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3668,7 +4082,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -3764,88 +4178,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:A13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>